<commit_message>
Generacion especificacion profiles y examples recursos Medication, Device y Specimen.
Generación especificación profiles y examples recursos Medication, Device y Specimen.
</commit_message>
<xml_diff>
--- a/fhir/indisa/StructureDefinition-AvailableTelemedicine.xlsx
+++ b/fhir/indisa/StructureDefinition-AvailableTelemedicine.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="70">
   <si>
     <t>Path</t>
   </si>
@@ -137,10 +137,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Admite telemedicina:</t>
-  </si>
-  <si>
-    <t>An Extension</t>
+    <t>Admit telemedicine</t>
+  </si>
+  <si>
+    <t>Active agenda for telemedicine care.</t>
   </si>
   <si>
     <t>*</t>
@@ -180,6 +180,9 @@
 </t>
   </si>
   <si>
+    <t>An Extension</t>
+  </si>
+  <si>
     <t xml:space="preserve">value:url}
 </t>
   </si>
@@ -209,7 +212,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>https://digitalware-klinic.github.io/fhir/indisa/StructureDefinition/AvailableTelemedicine</t>
+    <t>https://digitalware-klinic.github.io/fhir/indisa/StructureDefinition-AvailableTelemedicine</t>
   </si>
   <si>
     <t>N/A</t>
@@ -387,42 +390,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.59375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.16796875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.07421875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="37.171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="36.2890625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="19.625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="18.18359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="19.796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="17.6015625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="17.44140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="24.9765625" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="22.67578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -766,7 +769,7 @@
         <v>36</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -805,19 +808,19 @@
         <v>37</v>
       </c>
       <c r="AA4" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AB4" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AC4" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD4" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AE4" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AF4" t="s" s="2">
         <v>38</v>
@@ -837,7 +840,7 @@
     </row>
     <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
@@ -860,16 +863,16 @@
         <v>37</v>
       </c>
       <c r="J5" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" t="s" s="2">
@@ -877,7 +880,7 @@
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="R5" t="s" s="2">
         <v>37</v>
@@ -919,7 +922,7 @@
         <v>37</v>
       </c>
       <c r="AE5" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AF5" t="s" s="2">
         <v>39</v>
@@ -934,12 +937,12 @@
         <v>37</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" t="s" s="2">
@@ -962,13 +965,13 @@
         <v>37</v>
       </c>
       <c r="J6" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -1019,7 +1022,7 @@
         <v>37</v>
       </c>
       <c r="AE6" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AF6" t="s" s="2">
         <v>38</v>
@@ -1031,10 +1034,10 @@
         <v>37</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>